<commit_message>
added merging data from site and users
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -482,14 +482,12 @@
           <t>481289748</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
+      <c r="D2" t="n">
+        <v>85</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>officer</t>
+          <t>Member</t>
         </is>
       </c>
       <c r="F2" t="n">

</xml_diff>

<commit_message>
finished xlsx file. Added func fro edit. Started discord bot
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="09.09.2023" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="16.09.2023" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,6 +421,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="4" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -449,17 +461,17 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Average Energy</t>
+          <t>Energy</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Active Guild War</t>
+          <t>GW</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Active Battles</t>
+          <t>TW</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -495,6 +507,120 @@
       </c>
       <c r="G2" t="n">
         <v>9</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>фениксы, доктор афра</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="4" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Galactic Power</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Player ID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>GW</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Achernarkh Sun</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5289820</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>481289748</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>85</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Member</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>600</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8</v>
       </c>
       <c r="H2" t="n">
         <v>9</v>

</xml_diff>